<commit_message>
Modificaciones en los valores de la tabla del template, y ajuste de formato numérico en exportación a Excel
</commit_message>
<xml_diff>
--- a/merged_template.xlsx
+++ b/merged_template.xlsx
@@ -55,7 +55,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -63,7 +63,7 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -72,8 +72,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -458,7 +462,7 @@
           <t>Referencia / Factura</t>
         </is>
       </c>
-      <c r="E18" s="3" t="inlineStr">
+      <c r="E18" s="8" t="inlineStr">
         <is>
           <t>Importe de factura</t>
         </is>
@@ -473,7 +477,7 @@
           <t>Motivo del descuento</t>
         </is>
       </c>
-      <c r="H18" s="3" t="inlineStr">
+      <c r="H18" s="8" t="inlineStr">
         <is>
           <t>Pago Neto</t>
         </is>
@@ -495,12 +499,12 @@
           <t>PMP1243434</t>
         </is>
       </c>
-      <c r="E19" s="6" t="n">
+      <c r="E19" s="9" t="n">
         <v>165989699</v>
       </c>
       <c r="F19" s="5" t="inlineStr"/>
       <c r="G19" s="5" t="inlineStr"/>
-      <c r="H19" s="6" t="n">
+      <c r="H19" s="9" t="n">
         <v>165989699</v>
       </c>
       <c r="I19" s="7" t="inlineStr"/>
@@ -516,12 +520,12 @@
           <t>PMP1243435</t>
         </is>
       </c>
-      <c r="E20" s="6" t="n">
+      <c r="E20" s="9" t="n">
         <v>29856410</v>
       </c>
       <c r="F20" s="5" t="inlineStr"/>
       <c r="G20" s="5" t="inlineStr"/>
-      <c r="H20" s="6" t="n">
+      <c r="H20" s="9" t="n">
         <v>29856410</v>
       </c>
       <c r="I20" s="7" t="inlineStr"/>
@@ -537,12 +541,12 @@
           <t>PMP1243436</t>
         </is>
       </c>
-      <c r="E21" s="6" t="n">
+      <c r="E21" s="9" t="n">
         <v>12528130</v>
       </c>
       <c r="F21" s="5" t="inlineStr"/>
       <c r="G21" s="5" t="inlineStr"/>
-      <c r="H21" s="6" t="n">
+      <c r="H21" s="9" t="n">
         <v>12528130</v>
       </c>
       <c r="I21" s="7" t="inlineStr"/>
@@ -558,12 +562,12 @@
           <t>PMP1243437</t>
         </is>
       </c>
-      <c r="E22" s="6" t="n">
+      <c r="E22" s="9" t="n">
         <v>83124</v>
       </c>
       <c r="F22" s="5" t="inlineStr"/>
       <c r="G22" s="5" t="inlineStr"/>
-      <c r="H22" s="6" t="n">
+      <c r="H22" s="9" t="n">
         <v>83124</v>
       </c>
       <c r="I22" s="7" t="inlineStr"/>
@@ -579,12 +583,12 @@
           <t>PMP1243438</t>
         </is>
       </c>
-      <c r="E23" s="6" t="n">
+      <c r="E23" s="9" t="n">
         <v>53514044</v>
       </c>
       <c r="F23" s="5" t="inlineStr"/>
       <c r="G23" s="5" t="inlineStr"/>
-      <c r="H23" s="6" t="n">
+      <c r="H23" s="9" t="n">
         <v>53514044</v>
       </c>
       <c r="I23" s="7" t="inlineStr"/>
@@ -600,12 +604,12 @@
           <t>PMP1243439</t>
         </is>
       </c>
-      <c r="E24" s="6" t="n">
+      <c r="E24" s="9" t="n">
         <v>757032037</v>
       </c>
       <c r="F24" s="5" t="inlineStr"/>
       <c r="G24" s="5" t="inlineStr"/>
-      <c r="H24" s="6" t="n">
+      <c r="H24" s="9" t="n">
         <v>757032037</v>
       </c>
       <c r="I24" s="7" t="inlineStr"/>
@@ -621,12 +625,12 @@
           <t>PMP1243546</t>
         </is>
       </c>
-      <c r="E25" s="6" t="n">
+      <c r="E25" s="9" t="n">
         <v>122759901</v>
       </c>
       <c r="F25" s="5" t="inlineStr"/>
       <c r="G25" s="5" t="inlineStr"/>
-      <c r="H25" s="6" t="n">
+      <c r="H25" s="9" t="n">
         <v>122759901</v>
       </c>
       <c r="I25" s="7" t="inlineStr"/>
@@ -642,12 +646,12 @@
           <t>PMP1243587</t>
         </is>
       </c>
-      <c r="E26" s="6" t="n">
+      <c r="E26" s="9" t="n">
         <v>132622525</v>
       </c>
       <c r="F26" s="5" t="inlineStr"/>
       <c r="G26" s="5" t="inlineStr"/>
-      <c r="H26" s="6" t="n">
+      <c r="H26" s="9" t="n">
         <v>132622525</v>
       </c>
       <c r="I26" s="7" t="inlineStr"/>
@@ -663,12 +667,12 @@
           <t>PMP1243639</t>
         </is>
       </c>
-      <c r="E27" s="6" t="n">
+      <c r="E27" s="9" t="n">
         <v>343873745</v>
       </c>
       <c r="F27" s="5" t="inlineStr"/>
       <c r="G27" s="5" t="inlineStr"/>
-      <c r="H27" s="6" t="n">
+      <c r="H27" s="9" t="n">
         <v>343873745</v>
       </c>
       <c r="I27" s="7" t="inlineStr"/>
@@ -684,7 +688,7 @@
           <t>0085489002</t>
         </is>
       </c>
-      <c r="E28" s="6" t="n">
+      <c r="E28" s="9" t="n">
         <v>-106616</v>
       </c>
       <c r="F28" s="5" t="inlineStr">
@@ -697,7 +701,7 @@
           <t>987</t>
         </is>
       </c>
-      <c r="H28" s="6" t="n">
+      <c r="H28" s="9" t="n">
         <v>-106616</v>
       </c>
       <c r="I28" s="7" t="inlineStr">
@@ -717,7 +721,7 @@
           <t>0085489003</t>
         </is>
       </c>
-      <c r="E29" s="6" t="n">
+      <c r="E29" s="9" t="n">
         <v>-280732</v>
       </c>
       <c r="F29" s="5" t="inlineStr">
@@ -730,7 +734,7 @@
           <t>987</t>
         </is>
       </c>
-      <c r="H29" s="6" t="n">
+      <c r="H29" s="9" t="n">
         <v>-280732</v>
       </c>
       <c r="I29" s="7" t="inlineStr">
@@ -750,7 +754,7 @@
           <t>0085489004</t>
         </is>
       </c>
-      <c r="E30" s="6" t="n">
+      <c r="E30" s="9" t="n">
         <v>-852931</v>
       </c>
       <c r="F30" s="5" t="inlineStr">
@@ -763,7 +767,7 @@
           <t>987</t>
         </is>
       </c>
-      <c r="H30" s="6" t="n">
+      <c r="H30" s="9" t="n">
         <v>-852931</v>
       </c>
       <c r="I30" s="7" t="inlineStr">
@@ -783,7 +787,7 @@
           <t>0085489005</t>
         </is>
       </c>
-      <c r="E31" s="6" t="n">
+      <c r="E31" s="9" t="n">
         <v>-1235221</v>
       </c>
       <c r="F31" s="5" t="inlineStr">
@@ -796,7 +800,7 @@
           <t>987</t>
         </is>
       </c>
-      <c r="H31" s="6" t="n">
+      <c r="H31" s="9" t="n">
         <v>-1235221</v>
       </c>
       <c r="I31" s="7" t="inlineStr">
@@ -816,7 +820,7 @@
           <t>0085489006</t>
         </is>
       </c>
-      <c r="E32" s="6" t="n">
+      <c r="E32" s="9" t="n">
         <v>-2772024</v>
       </c>
       <c r="F32" s="5" t="inlineStr">
@@ -829,7 +833,7 @@
           <t>987</t>
         </is>
       </c>
-      <c r="H32" s="6" t="n">
+      <c r="H32" s="9" t="n">
         <v>-2772024</v>
       </c>
       <c r="I32" s="7" t="inlineStr">
@@ -849,7 +853,7 @@
           <t>0085489007</t>
         </is>
       </c>
-      <c r="E33" s="6" t="n">
+      <c r="E33" s="9" t="n">
         <v>-3198490</v>
       </c>
       <c r="F33" s="5" t="inlineStr">
@@ -862,7 +866,7 @@
           <t>987</t>
         </is>
       </c>
-      <c r="H33" s="6" t="n">
+      <c r="H33" s="9" t="n">
         <v>-3198490</v>
       </c>
       <c r="I33" s="7" t="inlineStr">
@@ -882,7 +886,7 @@
           <t>0085489008</t>
         </is>
       </c>
-      <c r="E34" s="6" t="n">
+      <c r="E34" s="9" t="n">
         <v>-4472640</v>
       </c>
       <c r="F34" s="5" t="inlineStr">
@@ -895,7 +899,7 @@
           <t>987</t>
         </is>
       </c>
-      <c r="H34" s="6" t="n">
+      <c r="H34" s="9" t="n">
         <v>-4472640</v>
       </c>
       <c r="I34" s="7" t="inlineStr">
@@ -915,7 +919,7 @@
           <t>0085489009</t>
         </is>
       </c>
-      <c r="E35" s="6" t="n">
+      <c r="E35" s="9" t="n">
         <v>-4895525</v>
       </c>
       <c r="F35" s="5" t="inlineStr">
@@ -928,7 +932,7 @@
           <t>987</t>
         </is>
       </c>
-      <c r="H35" s="6" t="n">
+      <c r="H35" s="9" t="n">
         <v>-4895525</v>
       </c>
       <c r="I35" s="7" t="inlineStr">
@@ -948,7 +952,7 @@
           <t>0085489010</t>
         </is>
       </c>
-      <c r="E36" s="6" t="n">
+      <c r="E36" s="9" t="n">
         <v>-6266272</v>
       </c>
       <c r="F36" s="5" t="inlineStr">
@@ -961,7 +965,7 @@
           <t>987</t>
         </is>
       </c>
-      <c r="H36" s="6" t="n">
+      <c r="H36" s="9" t="n">
         <v>-6266272</v>
       </c>
       <c r="I36" s="7" t="inlineStr">
@@ -981,7 +985,7 @@
           <t>0085489011</t>
         </is>
       </c>
-      <c r="E37" s="6" t="n">
+      <c r="E37" s="9" t="n">
         <v>-7156225</v>
       </c>
       <c r="F37" s="5" t="inlineStr">
@@ -994,7 +998,7 @@
           <t>987</t>
         </is>
       </c>
-      <c r="H37" s="6" t="n">
+      <c r="H37" s="9" t="n">
         <v>-7156225</v>
       </c>
       <c r="I37" s="7" t="inlineStr">
@@ -1014,7 +1018,7 @@
           <t>0085489012</t>
         </is>
       </c>
-      <c r="E38" s="6" t="n">
+      <c r="E38" s="9" t="n">
         <v>-7343319</v>
       </c>
       <c r="F38" s="5" t="inlineStr">
@@ -1027,7 +1031,7 @@
           <t>987</t>
         </is>
       </c>
-      <c r="H38" s="6" t="n">
+      <c r="H38" s="9" t="n">
         <v>-7343319</v>
       </c>
       <c r="I38" s="7" t="inlineStr">
@@ -1047,7 +1051,7 @@
           <t>0085489013</t>
         </is>
       </c>
-      <c r="E39" s="6" t="n">
+      <c r="E39" s="9" t="n">
         <v>-16267041</v>
       </c>
       <c r="F39" s="5" t="inlineStr">
@@ -1060,7 +1064,7 @@
           <t>987</t>
         </is>
       </c>
-      <c r="H39" s="6" t="n">
+      <c r="H39" s="9" t="n">
         <v>-16267041</v>
       </c>
       <c r="I39" s="7" t="inlineStr">
@@ -1080,7 +1084,7 @@
           <t>0085489014</t>
         </is>
       </c>
-      <c r="E40" s="6" t="n">
+      <c r="E40" s="9" t="n">
         <v>-19679618</v>
       </c>
       <c r="F40" s="5" t="inlineStr">
@@ -1093,7 +1097,7 @@
           <t>987</t>
         </is>
       </c>
-      <c r="H40" s="6" t="n">
+      <c r="H40" s="9" t="n">
         <v>-19679618</v>
       </c>
       <c r="I40" s="7" t="inlineStr">
@@ -1113,7 +1117,7 @@
           <t>0085489015</t>
         </is>
       </c>
-      <c r="E41" s="6" t="n">
+      <c r="E41" s="9" t="n">
         <v>-22519415</v>
       </c>
       <c r="F41" s="5" t="inlineStr">
@@ -1126,7 +1130,7 @@
           <t>987</t>
         </is>
       </c>
-      <c r="H41" s="6" t="n">
+      <c r="H41" s="9" t="n">
         <v>-22519415</v>
       </c>
       <c r="I41" s="7" t="inlineStr">
@@ -1146,7 +1150,7 @@
           <t>0085489016</t>
         </is>
       </c>
-      <c r="E42" s="6" t="n">
+      <c r="E42" s="9" t="n">
         <v>-24608350</v>
       </c>
       <c r="F42" s="5" t="inlineStr">
@@ -1159,7 +1163,7 @@
           <t>987</t>
         </is>
       </c>
-      <c r="H42" s="6" t="n">
+      <c r="H42" s="9" t="n">
         <v>-24608350</v>
       </c>
       <c r="I42" s="7" t="inlineStr">
@@ -1179,7 +1183,7 @@
           <t>0085489017</t>
         </is>
       </c>
-      <c r="E43" s="6" t="n">
+      <c r="E43" s="9" t="n">
         <v>-63642284</v>
       </c>
       <c r="F43" s="5" t="inlineStr">
@@ -1192,7 +1196,7 @@
           <t>987</t>
         </is>
       </c>
-      <c r="H43" s="6" t="n">
+      <c r="H43" s="9" t="n">
         <v>-63642284</v>
       </c>
       <c r="I43" s="7" t="inlineStr">
@@ -1212,7 +1216,7 @@
           <t>0085489018</t>
         </is>
       </c>
-      <c r="E44" s="6" t="n">
+      <c r="E44" s="9" t="n">
         <v>-77643586</v>
       </c>
       <c r="F44" s="5" t="inlineStr">
@@ -1225,7 +1229,7 @@
           <t>987</t>
         </is>
       </c>
-      <c r="H44" s="6" t="n">
+      <c r="H44" s="9" t="n">
         <v>-77643586</v>
       </c>
       <c r="I44" s="7" t="inlineStr">
@@ -1245,7 +1249,7 @@
           <t>0085489642</t>
         </is>
       </c>
-      <c r="E45" s="6" t="n">
+      <c r="E45" s="9" t="n">
         <v>-38727613</v>
       </c>
       <c r="F45" s="5" t="inlineStr">
@@ -1258,7 +1262,7 @@
           <t>987</t>
         </is>
       </c>
-      <c r="H45" s="6" t="n">
+      <c r="H45" s="9" t="n">
         <v>-38727613</v>
       </c>
       <c r="I45" s="7" t="inlineStr">
@@ -1278,7 +1282,7 @@
           <t>4631066394</t>
         </is>
       </c>
-      <c r="E46" s="6" t="n">
+      <c r="E46" s="9" t="n">
         <v>-35833</v>
       </c>
       <c r="F46" s="5" t="inlineStr">
@@ -1291,7 +1295,7 @@
           <t>522</t>
         </is>
       </c>
-      <c r="H46" s="6" t="n">
+      <c r="H46" s="9" t="n">
         <v>-35833</v>
       </c>
       <c r="I46" s="7" t="inlineStr">
@@ -1311,7 +1315,7 @@
           <t>4633043274</t>
         </is>
       </c>
-      <c r="E47" s="6" t="n">
+      <c r="E47" s="9" t="n">
         <v>-107500</v>
       </c>
       <c r="F47" s="5" t="inlineStr">
@@ -1324,7 +1328,7 @@
           <t>522</t>
         </is>
       </c>
-      <c r="H47" s="6" t="n">
+      <c r="H47" s="9" t="n">
         <v>-107500</v>
       </c>
       <c r="I47" s="7" t="inlineStr">
@@ -1344,7 +1348,7 @@
           <t>4633141222</t>
         </is>
       </c>
-      <c r="E48" s="6" t="n">
+      <c r="E48" s="9" t="n">
         <v>-31860</v>
       </c>
       <c r="F48" s="5" t="inlineStr">
@@ -1357,7 +1361,7 @@
           <t>522</t>
         </is>
       </c>
-      <c r="H48" s="6" t="n">
+      <c r="H48" s="9" t="n">
         <v>-31860</v>
       </c>
       <c r="I48" s="7" t="inlineStr">
@@ -1377,7 +1381,7 @@
           <t>4633373549</t>
         </is>
       </c>
-      <c r="E49" s="6" t="n">
+      <c r="E49" s="9" t="n">
         <v>-29575</v>
       </c>
       <c r="F49" s="5" t="inlineStr">
@@ -1390,7 +1394,7 @@
           <t>522</t>
         </is>
       </c>
-      <c r="H49" s="6" t="n">
+      <c r="H49" s="9" t="n">
         <v>-29575</v>
       </c>
       <c r="I49" s="7" t="inlineStr">
@@ -1410,7 +1414,7 @@
           <t>9801649295</t>
         </is>
       </c>
-      <c r="E50" s="6" t="n">
+      <c r="E50" s="9" t="n">
         <v>-817632</v>
       </c>
       <c r="F50" s="5" t="inlineStr">
@@ -1423,7 +1427,7 @@
           <t>CSB</t>
         </is>
       </c>
-      <c r="H50" s="6" t="n">
+      <c r="H50" s="9" t="n">
         <v>-817632</v>
       </c>
       <c r="I50" s="7" t="inlineStr">
@@ -1443,7 +1447,7 @@
           <t>9801649296</t>
         </is>
       </c>
-      <c r="E51" s="6" t="n">
+      <c r="E51" s="9" t="n">
         <v>-817632</v>
       </c>
       <c r="F51" s="5" t="inlineStr">
@@ -1456,7 +1460,7 @@
           <t>CSB</t>
         </is>
       </c>
-      <c r="H51" s="6" t="n">
+      <c r="H51" s="9" t="n">
         <v>-817632</v>
       </c>
       <c r="I51" s="7" t="inlineStr">
@@ -1476,7 +1480,7 @@
           <t>9801649297</t>
         </is>
       </c>
-      <c r="E52" s="6" t="n">
+      <c r="E52" s="9" t="n">
         <v>-3353617</v>
       </c>
       <c r="F52" s="5" t="inlineStr">
@@ -1489,7 +1493,7 @@
           <t>CSB</t>
         </is>
       </c>
-      <c r="H52" s="6" t="n">
+      <c r="H52" s="9" t="n">
         <v>-3353617</v>
       </c>
       <c r="I52" s="7" t="inlineStr">
@@ -1509,7 +1513,7 @@
           <t>9801649298</t>
         </is>
       </c>
-      <c r="E53" s="6" t="n">
+      <c r="E53" s="9" t="n">
         <v>-13687887</v>
       </c>
       <c r="F53" s="5" t="inlineStr">
@@ -1522,7 +1526,7 @@
           <t>CSB</t>
         </is>
       </c>
-      <c r="H53" s="6" t="n">
+      <c r="H53" s="9" t="n">
         <v>-13687887</v>
       </c>
       <c r="I53" s="7" t="inlineStr">
@@ -1542,7 +1546,7 @@
           <t>9801649299</t>
         </is>
       </c>
-      <c r="E54" s="6" t="n">
+      <c r="E54" s="9" t="n">
         <v>-14589753</v>
       </c>
       <c r="F54" s="5" t="inlineStr">
@@ -1555,7 +1559,7 @@
           <t>CSB</t>
         </is>
       </c>
-      <c r="H54" s="6" t="n">
+      <c r="H54" s="9" t="n">
         <v>-14589753</v>
       </c>
       <c r="I54" s="7" t="inlineStr">
@@ -1575,7 +1579,7 @@
           <t>9801649300</t>
         </is>
       </c>
-      <c r="E55" s="6" t="n">
+      <c r="E55" s="9" t="n">
         <v>-16674003</v>
       </c>
       <c r="F55" s="5" t="inlineStr">
@@ -1588,7 +1592,7 @@
           <t>CSB</t>
         </is>
       </c>
-      <c r="H55" s="6" t="n">
+      <c r="H55" s="9" t="n">
         <v>-16674003</v>
       </c>
       <c r="I55" s="7" t="inlineStr">
@@ -1608,7 +1612,7 @@
           <t>9801649301</t>
         </is>
       </c>
-      <c r="E56" s="6" t="n">
+      <c r="E56" s="9" t="n">
         <v>-19800379</v>
       </c>
       <c r="F56" s="5" t="inlineStr">
@@ -1621,7 +1625,7 @@
           <t>CSB</t>
         </is>
       </c>
-      <c r="H56" s="6" t="n">
+      <c r="H56" s="9" t="n">
         <v>-19800379</v>
       </c>
       <c r="I56" s="7" t="inlineStr">
@@ -1641,7 +1645,7 @@
           <t>9801649302</t>
         </is>
       </c>
-      <c r="E57" s="6" t="n">
+      <c r="E57" s="9" t="n">
         <v>-21786554</v>
       </c>
       <c r="F57" s="5" t="inlineStr">
@@ -1654,7 +1658,7 @@
           <t>CSB</t>
         </is>
       </c>
-      <c r="H57" s="6" t="n">
+      <c r="H57" s="9" t="n">
         <v>-21786554</v>
       </c>
       <c r="I57" s="7" t="inlineStr">
@@ -1674,7 +1678,7 @@
           <t>9801649303</t>
         </is>
       </c>
-      <c r="E58" s="6" t="n">
+      <c r="E58" s="9" t="n">
         <v>-47451687</v>
       </c>
       <c r="F58" s="5" t="inlineStr">
@@ -1687,7 +1691,7 @@
           <t>CSB</t>
         </is>
       </c>
-      <c r="H58" s="6" t="n">
+      <c r="H58" s="9" t="n">
         <v>-47451687</v>
       </c>
       <c r="I58" s="7" t="inlineStr">
@@ -1707,7 +1711,7 @@
           <t>9801649304</t>
         </is>
       </c>
-      <c r="E59" s="6" t="n">
+      <c r="E59" s="9" t="n">
         <v>-54866013</v>
       </c>
       <c r="F59" s="5" t="inlineStr">
@@ -1720,7 +1724,7 @@
           <t>CSB</t>
         </is>
       </c>
-      <c r="H59" s="6" t="n">
+      <c r="H59" s="9" t="n">
         <v>-54866013</v>
       </c>
       <c r="I59" s="7" t="inlineStr">
@@ -1740,7 +1744,7 @@
           <t>9801649305</t>
         </is>
       </c>
-      <c r="E60" s="6" t="n">
+      <c r="E60" s="9" t="n">
         <v>-65740358</v>
       </c>
       <c r="F60" s="5" t="inlineStr">
@@ -1753,7 +1757,7 @@
           <t>CSB</t>
         </is>
       </c>
-      <c r="H60" s="6" t="n">
+      <c r="H60" s="9" t="n">
         <v>-65740358</v>
       </c>
       <c r="I60" s="7" t="inlineStr">
@@ -1773,7 +1777,7 @@
           <t>PMP1243437</t>
         </is>
       </c>
-      <c r="E61" s="6" t="n">
+      <c r="E61" s="9" t="n">
         <v>-2</v>
       </c>
       <c r="F61" s="5" t="inlineStr">
@@ -1781,8 +1785,12 @@
           <t>RECHAZO</t>
         </is>
       </c>
-      <c r="G61" s="5" t="inlineStr"/>
-      <c r="H61" s="6" t="n">
+      <c r="G61" s="5" t="inlineStr">
+        <is>
+          <t>551</t>
+        </is>
+      </c>
+      <c r="H61" s="9" t="n">
         <v>-2</v>
       </c>
       <c r="I61" s="7" t="inlineStr">
@@ -1802,7 +1810,7 @@
           <t>PMP1243438</t>
         </is>
       </c>
-      <c r="E62" s="6" t="n">
+      <c r="E62" s="9" t="n">
         <v>-143069</v>
       </c>
       <c r="F62" s="5" t="inlineStr">
@@ -1810,8 +1818,12 @@
           <t>RECHAZO</t>
         </is>
       </c>
-      <c r="G62" s="5" t="inlineStr"/>
-      <c r="H62" s="6" t="n">
+      <c r="G62" s="5" t="inlineStr">
+        <is>
+          <t>551</t>
+        </is>
+      </c>
+      <c r="H62" s="9" t="n">
         <v>-143069</v>
       </c>
       <c r="I62" s="7" t="inlineStr">
@@ -1831,7 +1843,7 @@
           <t>PMP1243439</t>
         </is>
       </c>
-      <c r="E63" s="6" t="n">
+      <c r="E63" s="9" t="n">
         <v>-9553281</v>
       </c>
       <c r="F63" s="5" t="inlineStr">
@@ -1839,8 +1851,12 @@
           <t>RECHAZO</t>
         </is>
       </c>
-      <c r="G63" s="5" t="inlineStr"/>
-      <c r="H63" s="6" t="n">
+      <c r="G63" s="5" t="inlineStr">
+        <is>
+          <t>551</t>
+        </is>
+      </c>
+      <c r="H63" s="9" t="n">
         <v>-9553281</v>
       </c>
       <c r="I63" s="7" t="inlineStr">
@@ -1860,7 +1876,7 @@
           <t>PMP1243546</t>
         </is>
       </c>
-      <c r="E64" s="6" t="n">
+      <c r="E64" s="9" t="n">
         <v>-97382</v>
       </c>
       <c r="F64" s="5" t="inlineStr">
@@ -1868,8 +1884,12 @@
           <t>RECHAZO</t>
         </is>
       </c>
-      <c r="G64" s="5" t="inlineStr"/>
-      <c r="H64" s="6" t="n">
+      <c r="G64" s="5" t="inlineStr">
+        <is>
+          <t>551</t>
+        </is>
+      </c>
+      <c r="H64" s="9" t="n">
         <v>-97382</v>
       </c>
       <c r="I64" s="7" t="inlineStr">
@@ -1889,7 +1909,7 @@
           <t>PMP1243639</t>
         </is>
       </c>
-      <c r="E65" s="6" t="n">
+      <c r="E65" s="9" t="n">
         <v>-649</v>
       </c>
       <c r="F65" s="5" t="inlineStr">
@@ -1897,8 +1917,12 @@
           <t>RECHAZO</t>
         </is>
       </c>
-      <c r="G65" s="5" t="inlineStr"/>
-      <c r="H65" s="6" t="n">
+      <c r="G65" s="5" t="inlineStr">
+        <is>
+          <t>551</t>
+        </is>
+      </c>
+      <c r="H65" s="9" t="n">
         <v>-649</v>
       </c>
       <c r="I65" s="7" t="inlineStr">
@@ -1918,8 +1942,8 @@
           <t>PMP1243434</t>
         </is>
       </c>
-      <c r="E66" s="6" t="n">
-        <v>-38.15999999642372</v>
+      <c r="E66" s="9" t="n">
+        <v>38.15999999642372</v>
       </c>
       <c r="F66" s="5" t="inlineStr">
         <is>
@@ -1928,11 +1952,11 @@
       </c>
       <c r="G66" s="5" t="inlineStr">
         <is>
-          <t>WOB</t>
-        </is>
-      </c>
-      <c r="H66" s="6" t="n">
-        <v>-38.15999999642372</v>
+          <t>384</t>
+        </is>
+      </c>
+      <c r="H66" s="9" t="n">
+        <v>38.15999999642372</v>
       </c>
       <c r="I66" s="7" t="inlineStr">
         <is>
@@ -1951,8 +1975,8 @@
           <t>PMP1243435</t>
         </is>
       </c>
-      <c r="E67" s="6" t="n">
-        <v>0.2399999983608723</v>
+      <c r="E67" s="9" t="n">
+        <v>-0.2399999983608723</v>
       </c>
       <c r="F67" s="5" t="inlineStr">
         <is>
@@ -1961,11 +1985,11 @@
       </c>
       <c r="G67" s="5" t="inlineStr">
         <is>
-          <t>384</t>
-        </is>
-      </c>
-      <c r="H67" s="6" t="n">
-        <v>0.2399999983608723</v>
+          <t>WOB</t>
+        </is>
+      </c>
+      <c r="H67" s="9" t="n">
+        <v>-0.2399999983608723</v>
       </c>
       <c r="I67" s="7" t="inlineStr">
         <is>
@@ -1984,8 +2008,8 @@
           <t>PMP1243437</t>
         </is>
       </c>
-      <c r="E68" s="6" t="n">
-        <v>-0.5</v>
+      <c r="E68" s="9" t="n">
+        <v>0.5</v>
       </c>
       <c r="F68" s="5" t="inlineStr">
         <is>
@@ -1994,11 +2018,11 @@
       </c>
       <c r="G68" s="5" t="inlineStr">
         <is>
-          <t>WOB</t>
-        </is>
-      </c>
-      <c r="H68" s="6" t="n">
-        <v>-0.5</v>
+          <t>384</t>
+        </is>
+      </c>
+      <c r="H68" s="9" t="n">
+        <v>0.5</v>
       </c>
       <c r="I68" s="7" t="inlineStr">
         <is>
@@ -2017,8 +2041,8 @@
           <t>PMP1243438</t>
         </is>
       </c>
-      <c r="E69" s="6" t="n">
-        <v>-0.2800000011920929</v>
+      <c r="E69" s="9" t="n">
+        <v>0.2800000011920929</v>
       </c>
       <c r="F69" s="5" t="inlineStr">
         <is>
@@ -2027,11 +2051,11 @@
       </c>
       <c r="G69" s="5" t="inlineStr">
         <is>
-          <t>WOB</t>
-        </is>
-      </c>
-      <c r="H69" s="6" t="n">
-        <v>-0.2800000011920929</v>
+          <t>384</t>
+        </is>
+      </c>
+      <c r="H69" s="9" t="n">
+        <v>0.2800000011920929</v>
       </c>
       <c r="I69" s="7" t="inlineStr">
         <is>
@@ -2050,8 +2074,8 @@
           <t>PMP1243439</t>
         </is>
       </c>
-      <c r="E70" s="6" t="n">
-        <v>0.2200000286102295</v>
+      <c r="E70" s="9" t="n">
+        <v>-0.2200000286102295</v>
       </c>
       <c r="F70" s="5" t="inlineStr">
         <is>
@@ -2060,11 +2084,11 @@
       </c>
       <c r="G70" s="5" t="inlineStr">
         <is>
-          <t>384</t>
-        </is>
-      </c>
-      <c r="H70" s="6" t="n">
-        <v>0.2200000286102295</v>
+          <t>WOB</t>
+        </is>
+      </c>
+      <c r="H70" s="9" t="n">
+        <v>-0.2200000286102295</v>
       </c>
       <c r="I70" s="7" t="inlineStr">
         <is>
@@ -2083,8 +2107,8 @@
           <t>PMP1243546</t>
         </is>
       </c>
-      <c r="E71" s="6" t="n">
-        <v>1.700000002980232</v>
+      <c r="E71" s="9" t="n">
+        <v>-1.700000002980232</v>
       </c>
       <c r="F71" s="5" t="inlineStr">
         <is>
@@ -2093,46 +2117,46 @@
       </c>
       <c r="G71" s="5" t="inlineStr">
         <is>
+          <t>WOB</t>
+        </is>
+      </c>
+      <c r="H71" s="9" t="n">
+        <v>-1.700000002980232</v>
+      </c>
+      <c r="I71" s="7" t="inlineStr">
+        <is>
+          <t>MENORES VALORES PMP1243546</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="C72" s="5" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D72" s="5" t="inlineStr">
+        <is>
+          <t>PMP1243639</t>
+        </is>
+      </c>
+      <c r="E72" s="9" t="n">
+        <v>0.9399999976158142</v>
+      </c>
+      <c r="F72" s="5" t="inlineStr">
+        <is>
+          <t>MENORES VALORES</t>
+        </is>
+      </c>
+      <c r="G72" s="5" t="inlineStr">
+        <is>
           <t>384</t>
         </is>
       </c>
-      <c r="H71" s="6" t="n">
-        <v>1.700000002980232</v>
-      </c>
-      <c r="I71" s="7" t="inlineStr">
-        <is>
-          <t>MENORES VALORES PMP1243546</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>PMP1243639</t>
-        </is>
-      </c>
-      <c r="E72" t="n">
-        <v>-0.9399999976158142</v>
-      </c>
-      <c r="F72" t="inlineStr">
-        <is>
-          <t>MENORES VALORES</t>
-        </is>
-      </c>
-      <c r="G72" t="inlineStr">
-        <is>
-          <t>WOB</t>
-        </is>
-      </c>
-      <c r="H72" t="n">
-        <v>-0.9399999976158142</v>
-      </c>
-      <c r="I72" t="inlineStr">
+      <c r="H72" s="9" t="n">
+        <v>0.9399999976158142</v>
+      </c>
+      <c r="I72" s="7" t="inlineStr">
         <is>
           <t>MENORES VALORES PMP1243639</t>
         </is>

</xml_diff>